<commit_message>
* Add Jack Kuipers to Core LOC * Move Committees to About Tab
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514536E1-52CD-4ED8-821B-EA76AAB2BC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10EE269-A853-4455-B520-B3853A87C61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1227,7 +1227,9 @@
         <v>45</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
       <c r="F17" s="4">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
* Add Diane Uschner * Add full name for Bibiana Blatna * Add affiliations
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10EE269-A853-4455-B520-B3853A87C61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C0DE36-5E0E-4A7B-AA6D-74B3D65CCC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
+    <workbookView xWindow="13830" yWindow="2610" windowWidth="24165" windowHeight="14160" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="132">
   <si>
     <t>first</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Pasquale</t>
   </si>
   <si>
-    <t>Bibi</t>
-  </si>
-  <si>
     <t>Blatna</t>
   </si>
   <si>
@@ -421,6 +418,15 @@
   </si>
   <si>
     <t>BIPS</t>
+  </si>
+  <si>
+    <t>Bibiana</t>
+  </si>
+  <si>
+    <t>Diane</t>
+  </si>
+  <si>
+    <t>Uschner</t>
   </si>
 </sst>
 </file>
@@ -852,28 +858,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="46.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.84375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.3046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.3046875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.3828125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.84375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.84375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.53515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.53515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="46.84375" style="7"/>
+    <col min="2" max="2" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="46.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -896,16 +902,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -916,7 +922,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -931,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -942,7 +948,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -957,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -968,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4">
@@ -979,7 +985,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1022,7 +1028,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1040,7 +1046,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1058,7 +1064,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1076,7 +1082,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1096,7 +1102,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1116,7 +1122,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1136,7 +1142,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1156,7 +1162,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1176,12 +1182,12 @@
       <c r="G14" s="4"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
@@ -1196,12 +1202,12 @@
       <c r="G15" s="4"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
@@ -1216,15 +1222,15 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4">
@@ -1236,12 +1242,12 @@
       <c r="G17" s="4"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -1254,12 +1260,12 @@
       <c r="G18" s="4"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
@@ -1272,12 +1278,12 @@
       <c r="G19" s="4"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>17</v>
@@ -1290,12 +1296,12 @@
       <c r="G20" s="4"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>36</v>
@@ -1308,12 +1314,12 @@
       <c r="G21" s="4"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>27</v>
@@ -1326,12 +1332,12 @@
       <c r="G22" s="4"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
@@ -1344,15 +1350,15 @@
       <c r="G23" s="4"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -1362,12 +1368,12 @@
       <c r="G24" s="4"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>14</v>
@@ -1380,15 +1386,15 @@
       <c r="G25" s="4"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -1398,15 +1404,15 @@
       <c r="G26" s="4"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -1419,18 +1425,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1439,18 +1445,18 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1459,18 +1465,18 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1479,18 +1485,18 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1499,18 +1505,18 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1519,18 +1525,18 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1539,18 +1545,18 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1559,18 +1565,18 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1579,18 +1585,18 @@
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1599,18 +1605,18 @@
       </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1619,18 +1625,18 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1639,18 +1645,18 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -1659,18 +1665,18 @@
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -1679,18 +1685,18 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -1699,12 +1705,12 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>11</v>
@@ -1717,12 +1723,12 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>27</v>
@@ -1734,15 +1740,15 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="C44" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="6"/>
@@ -1752,12 +1758,12 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>27</v>
@@ -1769,23 +1775,37 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>116</v>
-      </c>
       <c r="C46" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G46" s="7">
         <v>1</v>
       </c>
       <c r="J46" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Add Baldur Magnusson
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C0DE36-5E0E-4A7B-AA6D-74B3D65CCC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97642C36-6D67-4B59-B8C2-6B144703673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13830" yWindow="2610" windowWidth="24165" windowHeight="14160" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="135">
   <si>
     <t>first</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t>Uschner</t>
+  </si>
+  <si>
+    <t>Baldur</t>
+  </si>
+  <si>
+    <t>Magnusson</t>
+  </si>
+  <si>
+    <t>UCB</t>
   </si>
 </sst>
 </file>
@@ -858,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +880,7 @@
     <col min="3" max="3" width="23.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
@@ -1679,7 +1688,6 @@
         <v>124</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
       <c r="G40" s="6">
         <v>1</v>
       </c>
@@ -1699,7 +1707,6 @@
         <v>118</v>
       </c>
       <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
       <c r="G41" s="6">
         <v>1</v>
       </c>
@@ -1805,7 +1812,21 @@
       <c r="C47" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F48" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: affiliation for Samuel M, Kelly VL, Katherine L, Paul G. Plus, changed the order on Niko name (first, last instead of last, first)
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97642C36-6D67-4B59-B8C2-6B144703673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B835AB56-2AEA-43BD-BBD5-58E95C07C465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13830" yWindow="2610" windowWidth="24165" windowHeight="14160" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
+    <workbookView xWindow="19090" yWindow="-10850" windowWidth="38620" windowHeight="21100" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,6 @@
     <t>Lee</t>
   </si>
   <si>
-    <t>Murdoch</t>
-  </si>
-  <si>
     <t>Paul</t>
   </si>
   <si>
@@ -339,9 +336,6 @@
     <t>Muller</t>
   </si>
   <si>
-    <t>U Macquarie</t>
-  </si>
-  <si>
     <t>Phillippo</t>
   </si>
   <si>
@@ -393,12 +387,6 @@
     <t>CH</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>NL</t>
-  </si>
-  <si>
     <t>EE</t>
   </si>
   <si>
@@ -436,6 +424,18 @@
   </si>
   <si>
     <t>UCB</t>
+  </si>
+  <si>
+    <t>Macquarie U</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>MCRI</t>
+  </si>
+  <si>
+    <t>CAN</t>
   </si>
 </sst>
 </file>
@@ -869,26 +869,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="46.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="46.85546875" style="7"/>
+    <col min="2" max="2" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="46.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -911,16 +911,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -931,7 +931,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -946,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -957,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -983,7 +983,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4">
@@ -994,7 +994,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1111,7 +1111,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1191,9 +1191,9 @@
       <c r="G14" s="4"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>39</v>
@@ -1211,7 +1211,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1231,7 +1231,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
@@ -1269,7 +1269,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>55</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -1377,7 +1377,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>67</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>69</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>72</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>75</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1494,18 +1494,18 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>78</v>
       </c>
@@ -1522,10 +1522,10 @@
         <v>79</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1534,18 +1534,18 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1554,18 +1554,18 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1574,18 +1574,18 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1594,18 +1594,18 @@
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1614,18 +1614,18 @@
       </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1634,18 +1634,18 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1654,18 +1654,18 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -1674,18 +1674,18 @@
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="C40" s="3" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E40" s="6"/>
       <c r="G40" s="6">
@@ -1693,18 +1693,18 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E41" s="6"/>
       <c r="G41" s="6">
@@ -1712,12 +1712,12 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>11</v>
@@ -1730,12 +1730,12 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>27</v>
@@ -1747,12 +1747,12 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>63</v>
@@ -1765,12 +1765,12 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>27</v>
@@ -1782,32 +1782,32 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D46" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1</v>
+      </c>
+      <c r="J46" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="G46" s="7">
-        <v>1</v>
-      </c>
-      <c r="J46" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>8</v>
@@ -1816,15 +1816,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F48" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
* Add key dates * Fix affiliations
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B835AB56-2AEA-43BD-BBD5-58E95C07C465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBF3D01-93C6-48D5-BDE4-A2CD2D4F71E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10850" windowWidth="38620" windowHeight="21100" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
     <t>MCRI</t>
   </si>
   <si>
-    <t>CAN</t>
+    <t>CA</t>
   </si>
 </sst>
 </file>
@@ -870,25 +870,25 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="46.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="46.88671875" style="7"/>
+    <col min="2" max="2" width="14.84375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.3046875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.84375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.84375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.53515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.53515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="46.84375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +920,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -946,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -994,7 +994,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1111,7 +1111,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>125</v>
       </c>
@@ -1211,7 +1211,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -1231,7 +1231,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
@@ -1269,7 +1269,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>55</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>67</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>77</v>
       </c>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>78</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>80</v>
       </c>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>83</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>88</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>90</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>93</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>96</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>99</v>
       </c>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>103</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
         <v>105</v>
       </c>
@@ -1747,7 +1747,7 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>107</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>109</v>
       </c>
@@ -1782,7 +1782,7 @@
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="7" t="s">
         <v>112</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="7" t="s">
         <v>126</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
* Change layout of fees
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2687C18E-F627-F145-B317-13BF8E6FEE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75F6B93-7F9A-5F41-895C-3B7A5119884A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="136">
   <si>
     <t>first</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Ross</t>
   </si>
   <si>
-    <t>Swiss TPH</t>
-  </si>
-  <si>
     <t>Muriel</t>
   </si>
   <si>
@@ -430,6 +427,18 @@
   </si>
   <si>
     <t>CA</t>
+  </si>
+  <si>
+    <t>Swiss TPH &amp; U Basel</t>
+  </si>
+  <si>
+    <t>DSM Firmenich</t>
+  </si>
+  <si>
+    <t>Merck</t>
+  </si>
+  <si>
+    <t>Cogitamen</t>
   </si>
 </sst>
 </file>
@@ -864,7 +873,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -893,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -905,13 +914,13 @@
         <v>5</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -922,10 +931,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -951,7 +960,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -977,7 +986,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4">
@@ -1075,7 +1084,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
@@ -1087,10 +1096,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
@@ -1107,10 +1116,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
@@ -1127,13 +1136,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4">
@@ -1147,13 +1156,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4">
@@ -1167,10 +1176,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
@@ -1187,10 +1196,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
@@ -1207,10 +1216,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
@@ -1227,13 +1236,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4">
@@ -1247,10 +1256,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -1265,10 +1274,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>8</v>
@@ -1283,10 +1292,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>17</v>
@@ -1301,13 +1310,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
@@ -1319,10 +1328,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -1337,13 +1346,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
@@ -1355,10 +1364,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>14</v>
@@ -1373,13 +1382,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
@@ -1391,13 +1400,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -1412,16 +1421,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1432,16 +1441,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1452,16 +1461,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1472,16 +1481,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1492,16 +1501,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1512,16 +1521,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1532,16 +1541,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1552,16 +1561,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1572,16 +1581,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1592,16 +1601,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1612,16 +1621,16 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1632,16 +1641,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1652,16 +1661,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C39" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E39" s="6"/>
       <c r="G39" s="6">
@@ -1674,13 +1683,13 @@
         <v>18</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E40" s="6"/>
       <c r="G40" s="6">
@@ -1690,10 +1699,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>11</v>
@@ -1708,13 +1717,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="C42" s="7" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="6">
@@ -1725,13 +1734,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="C43" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="6"/>
@@ -1743,13 +1752,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>27</v>
+      <c r="C44" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6">
@@ -1760,16 +1769,16 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="C45" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G45" s="7">
         <v>1</v>
@@ -1780,10 +1789,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>8</v>
@@ -1794,13 +1803,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="F47" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
* Update committee and affiliations * Short courses -> Pre-conference courses
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75F6B93-7F9A-5F41-895C-3B7A5119884A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6FC8B7-2344-B546-986A-E5E9499A6728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="139">
   <si>
     <t>first</t>
   </si>
@@ -439,6 +439,15 @@
   </si>
   <si>
     <t>Cogitamen</t>
+  </si>
+  <si>
+    <t>Marci</t>
+  </si>
+  <si>
+    <t>Rückbeil</t>
+  </si>
+  <si>
+    <t>Sanofi</t>
   </si>
 </sst>
 </file>
@@ -870,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1171,7 +1180,9 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1812,6 +1823,20 @@
         <v>127</v>
       </c>
       <c r="F47" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G48" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Add finance LOC member
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE41B342-733B-BB45-8279-AF5865543E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCABC84-5205-D743-B41E-F1D4939096BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="33120" windowHeight="18120" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="144">
   <si>
     <t>first</t>
   </si>
@@ -457,6 +457,12 @@
   </si>
   <si>
     <t>Philip Morris</t>
+  </si>
+  <si>
+    <t>Chantal</t>
+  </si>
+  <si>
+    <t>Meré</t>
   </si>
 </sst>
 </file>
@@ -888,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1859,7 +1865,27 @@
       <c r="C49" s="7" t="s">
         <v>141</v>
       </c>
+      <c r="F49" s="6">
+        <v>1</v>
+      </c>
       <c r="I49" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="6">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplify main page text and add supporting reviewers
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B222B58-220E-499A-ADFC-7744CA167442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DFC42B-54D5-1441-B876-9E426A67EF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24300" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="176">
   <si>
     <t>first</t>
   </si>
@@ -463,6 +463,102 @@
   </si>
   <si>
     <t>Charline</t>
+  </si>
+  <si>
+    <t>Björn</t>
+  </si>
+  <si>
+    <t>Bornkamp</t>
+  </si>
+  <si>
+    <t>Campbell</t>
+  </si>
+  <si>
+    <t>Dejardin</t>
+  </si>
+  <si>
+    <t>Devenport</t>
+  </si>
+  <si>
+    <t>Dukes</t>
+  </si>
+  <si>
+    <t>Dumas</t>
+  </si>
+  <si>
+    <t>EPFL</t>
+  </si>
+  <si>
+    <t>Goldberg</t>
+  </si>
+  <si>
+    <t>Technion</t>
+  </si>
+  <si>
+    <t>Magirr</t>
+  </si>
+  <si>
+    <t>Mercier</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>UCL</t>
+  </si>
+  <si>
+    <t>Remiro-Azocar</t>
+  </si>
+  <si>
+    <t>Novo Nordisk</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Tarr</t>
+  </si>
+  <si>
+    <t>U Sydney</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Harlan</t>
+  </si>
+  <si>
+    <t>Jenny</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Elise</t>
+  </si>
+  <si>
+    <t>Yair</t>
+  </si>
+  <si>
+    <t>Dominic Edmund</t>
+  </si>
+  <si>
+    <t>Francois</t>
+  </si>
+  <si>
+    <t>Tim P.</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Garth</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>sup_reviewer</t>
   </si>
 </sst>
 </file>
@@ -894,28 +990,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9503F084-95F7-412B-907D-317B16782585}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.84375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.3828125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.3828125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.3828125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.84375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.84375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3828125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.3828125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="46.84375" style="7"/>
+    <col min="1" max="1" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="46.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,8 +1043,11 @@
       <c r="J1" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -973,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -999,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1021,7 +1121,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1046,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1168,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1186,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1104,7 +1204,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1122,7 +1222,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1142,7 +1242,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -1162,7 +1262,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -1182,7 +1282,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -1204,7 +1304,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1224,7 +1324,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>121</v>
       </c>
@@ -1244,7 +1344,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1264,7 +1364,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1283,8 +1383,11 @@
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="K17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -1302,7 +1405,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1320,7 +1423,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
@@ -1338,7 +1441,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>49</v>
       </c>
@@ -1356,7 +1459,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -1374,7 +1477,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>53</v>
       </c>
@@ -1392,7 +1495,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
@@ -1410,7 +1513,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1531,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
@@ -1449,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>63</v>
       </c>
@@ -1469,7 +1572,7 @@
       </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
@@ -1489,7 +1592,7 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
@@ -1509,7 +1612,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
@@ -1529,7 +1632,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>74</v>
       </c>
@@ -1549,7 +1652,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>76</v>
       </c>
@@ -1569,7 +1672,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>79</v>
       </c>
@@ -1589,7 +1692,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
@@ -1609,7 +1712,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>84</v>
       </c>
@@ -1629,7 +1732,7 @@
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>86</v>
       </c>
@@ -1649,7 +1752,7 @@
       </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>89</v>
       </c>
@@ -1669,7 +1772,7 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>92</v>
       </c>
@@ -1689,7 +1792,7 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
@@ -1708,7 +1811,7 @@
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
@@ -1727,7 +1830,7 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>99</v>
       </c>
@@ -1745,7 +1848,7 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>101</v>
       </c>
@@ -1762,7 +1865,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>103</v>
       </c>
@@ -1780,7 +1883,7 @@
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>105</v>
       </c>
@@ -1797,7 +1900,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>108</v>
       </c>
@@ -1817,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>122</v>
       </c>
@@ -1831,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>124</v>
       </c>
@@ -1845,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>134</v>
       </c>
@@ -1859,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>137</v>
       </c>
@@ -1876,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>143</v>
       </c>
@@ -1890,6 +1993,227 @@
         <v>1</v>
       </c>
       <c r="I50" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K51" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="K52" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K54" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K55" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K56" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K57" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K58" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K59" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K60" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K61" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="K62" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K63" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Jack Kuipers country code
</commit_message>
<xml_diff>
--- a/data/committees.xlsx
+++ b/data/committees.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DFC42B-54D5-1441-B876-9E426A67EF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8354A0B-BABB-6C44-AAA5-EC6FA2905164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24300" xr2:uid="{6613D4AF-51BE-4917-B559-FB4362D11699}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="176">
   <si>
     <t>first</t>
   </si>
@@ -993,7 +993,7 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1374,7 +1374,9 @@
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E17" s="4">
         <v>1</v>
       </c>

</xml_diff>